<commit_message>
adicionado o inicio da janela de corrigir gabarito
</commit_message>
<xml_diff>
--- a/bancodedados/gabarito_teste4[Ciências Humanas].xlsx
+++ b/bancodedados/gabarito_teste4[Ciências Humanas].xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t xml:space="preserve">  E</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t xml:space="preserve">  C</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t xml:space="preserve">  B</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t xml:space="preserve">  B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t xml:space="preserve">  D</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t xml:space="preserve">  B</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>B</t>
+          <t xml:space="preserve">  B</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t xml:space="preserve">  D</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t xml:space="preserve">  E</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>E</t>
+          <t xml:space="preserve">  E</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>D</t>
+          <t xml:space="preserve">  D</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t xml:space="preserve">  C</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t xml:space="preserve">  D</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t xml:space="preserve">  B</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">  A</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">  A</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t xml:space="preserve">  C</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -706,7 +706,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>B</t>
+          <t xml:space="preserve">  B</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>C</t>
+          <t xml:space="preserve">  C</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -736,310 +736,10 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>C</t>
+          <t xml:space="preserve">  C</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>

</xml_diff>